<commit_message>
More review fixes and initial analysis
</commit_message>
<xml_diff>
--- a/revised reviews/CEP paper review form 2023_2024 revised.xlsx
+++ b/revised reviews/CEP paper review form 2023_2024 revised.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://durhamuniversity-my.sharepoint.com/personal/dcs0spb_durham_ac_uk/Documents/Pedagogy/Projects/CEP_Retro/revised reviews/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dcs0spb/Software/CEP_Retro/revised reviews/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="8_{16115E65-1032-DC49-A60E-AC05B557F745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{20DD6B71-9DDE-8B4F-A2EC-05BC41627A74}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1E472D-3B21-2C49-BF1A-E48E723EB0F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="140" yWindow="900" windowWidth="29920" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="132">
   <si>
     <t>Timestamp</t>
   </si>
@@ -509,9 +509,6 @@
   </si>
   <si>
     <t>new option</t>
-  </si>
-  <si>
-    <t>outreach not schools</t>
   </si>
   <si>
     <t>pathways</t>
@@ -1032,9 +1029,9 @@
   </sheetPr>
   <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1091,7 +1088,7 @@
         <v>11</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>12</v>
@@ -1842,10 +1839,10 @@
         <v>36</v>
       </c>
       <c r="K22" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="L22" s="16" t="s">
         <v>130</v>
-      </c>
-      <c r="L22" s="16" t="s">
-        <v>131</v>
       </c>
       <c r="M22" s="18"/>
       <c r="N22" s="18" t="s">
@@ -1884,10 +1881,10 @@
         <v>36</v>
       </c>
       <c r="K23" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="L23" s="13" t="s">
         <v>130</v>
-      </c>
-      <c r="L23" s="13" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="28" x14ac:dyDescent="0.15">
@@ -2059,7 +2056,7 @@
         <v>29</v>
       </c>
       <c r="K28" s="6" t="s">
-        <v>130</v>
+        <v>30</v>
       </c>
       <c r="L28" s="6" t="s">
         <v>96</v>
@@ -2097,7 +2094,7 @@
         <v>29</v>
       </c>
       <c r="K29" s="6" t="s">
-        <v>130</v>
+        <v>30</v>
       </c>
       <c r="L29" s="8" t="s">
         <v>96</v>

</xml_diff>

<commit_message>
Combined reviews, generated graphs and tables
</commit_message>
<xml_diff>
--- a/revised reviews/CEP paper review form 2023_2024 revised.xlsx
+++ b/revised reviews/CEP paper review form 2023_2024 revised.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dcs0spb/Software/CEP_Retro/revised reviews/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1E472D-3B21-2C49-BF1A-E48E723EB0F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{596900A5-7E38-FF4F-8F59-095B529BFF87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="140" yWindow="900" windowWidth="29920" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1030,8 +1030,8 @@
   <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K30" sqref="K30"/>
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1154,8 +1154,8 @@
       <c r="I3" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="16" t="s">
-        <v>16</v>
+      <c r="J3" s="13" t="s">
+        <v>20</v>
       </c>
       <c r="K3" s="16" t="s">
         <v>37</v>
@@ -2297,8 +2297,8 @@
       <c r="I35" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="J35" s="13" t="s">
-        <v>16</v>
+      <c r="J35" s="16" t="s">
+        <v>20</v>
       </c>
       <c r="K35" s="13" t="s">
         <v>21</v>

</xml_diff>